<commit_message>
1. Done code clean up and refactoring 2. Moved the reusable function to utility 3. Scenario 2 handled with excel instead of datatable values. 4. Removed excel data reading from Scenario 3, entering random values to fill form. 5. Replaced stream with loop
</commit_message>
<xml_diff>
--- a/src/main/resources/ExcelData/guestScenario.xlsx
+++ b/src/main/resources/ExcelData/guestScenario.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rejijoseph/Documents/Reji/Jisha/GlobalPayments/TechProject/SDETTII_Technical_Test/src/main/resources/ExcelData/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F68B57B5-9963-B14A-BE0B-0AF06B4F0571}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29CFF9A0-3476-8042-AAE4-7419F8D12D9A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="23260" windowHeight="12460" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="contactus" sheetId="1" r:id="rId1"/>
+    <sheet name="OptionsList" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,31 +25,25 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
-    <t>Contact Name</t>
+    <t>Options</t>
   </si>
   <si>
-    <t>Contact Email</t>
+    <t>Meat &amp; Fish</t>
   </si>
   <si>
-    <t>Contact Enquiry</t>
+    <t>Fruits &amp; Vegetables</t>
   </si>
   <si>
-    <t>More cart options</t>
-  </si>
-  <si>
-    <t>TestUser</t>
-  </si>
-  <si>
-    <t>testuser@test.com</t>
+    <t>Groceries</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -65,12 +59,11 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
+      <b/>
+      <sz val="9.8000000000000007"/>
+      <color rgb="FF297BDE"/>
+      <name val="JetBrains Mono"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="3">
@@ -96,17 +89,15 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -385,46 +376,39 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:A4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="J16" sqref="J16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="11.83203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:1" s="1" customFormat="1">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+    </row>
+    <row r="2" spans="1:1">
+      <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+    </row>
+    <row r="3" spans="1:1">
+      <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" t="s">
+    <row r="4" spans="1:1">
+      <c r="A4" s="2" t="s">
         <v>3</v>
       </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" xr:uid="{517C68F9-88E4-7B44-BB77-54DF611F599A}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>